<commit_message>
added primary, secondary standards to U-Pb table
</commit_message>
<xml_diff>
--- a/data/zircon_U-Pb/LASS ICPMS U-Pb.xlsx
+++ b/data/zircon_U-Pb/LASS ICPMS U-Pb.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian\Documents\manuscripts\Oman-paleomag-shaat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XPS\Documents\manuscripts\Oman-paleomag-shaat\2025_Oman_Paleogeography\data\zircon_U-Pb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3E2BB5-81A4-42EB-BD8B-F48C46D0C80A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE147A4E-8662-4B82-80A9-AB86173BD113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{B5398E37-5FD9-4359-82A2-774148DEAEDA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{B5398E37-5FD9-4359-82A2-774148DEAEDA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="samples" sheetId="1" r:id="rId1"/>
+    <sheet name="standards" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="63">
   <si>
     <t>Final Pb206/U238_mean</t>
   </si>
@@ -202,12 +203,36 @@
   <si>
     <t>S14</t>
   </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>GJ1</t>
+  </si>
+  <si>
+    <t>Mali</t>
+  </si>
+  <si>
+    <t>NIST612</t>
+  </si>
+  <si>
+    <t>OG</t>
+  </si>
+  <si>
+    <t>Piexe</t>
+  </si>
+  <si>
+    <t>Ples</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,6 +244,12 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -241,9 +272,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,36 +613,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC4D7E9A-363F-4D67-B5C5-CE9C5AAB0E79}">
   <dimension ref="A1:AA36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AD16" sqref="AD16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" customWidth="1"/>
-    <col min="6" max="6" width="29.28515625" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" customWidth="1"/>
+    <col min="4" max="4" width="27.109375" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" customWidth="1"/>
+    <col min="6" max="6" width="29.33203125" customWidth="1"/>
     <col min="7" max="7" width="22" customWidth="1"/>
-    <col min="8" max="8" width="25.7109375" customWidth="1"/>
-    <col min="9" max="9" width="25.85546875" customWidth="1"/>
-    <col min="10" max="10" width="29.140625" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" customWidth="1"/>
-    <col min="12" max="13" width="25.7109375" customWidth="1"/>
+    <col min="8" max="8" width="25.6640625" customWidth="1"/>
+    <col min="9" max="9" width="25.88671875" customWidth="1"/>
+    <col min="10" max="10" width="29.109375" customWidth="1"/>
+    <col min="11" max="11" width="23.44140625" customWidth="1"/>
+    <col min="12" max="13" width="25.6640625" customWidth="1"/>
     <col min="14" max="14" width="31" customWidth="1"/>
-    <col min="15" max="15" width="23.28515625" customWidth="1"/>
-    <col min="16" max="18" width="25.7109375" customWidth="1"/>
-    <col min="19" max="19" width="22.85546875" customWidth="1"/>
-    <col min="20" max="20" width="25.7109375" customWidth="1"/>
-    <col min="21" max="21" width="16.85546875" customWidth="1"/>
-    <col min="22" max="22" width="21.42578125" customWidth="1"/>
-    <col min="23" max="24" width="21.7109375" customWidth="1"/>
-    <col min="26" max="26" width="24.7109375" customWidth="1"/>
+    <col min="15" max="15" width="23.33203125" customWidth="1"/>
+    <col min="16" max="18" width="25.6640625" customWidth="1"/>
+    <col min="19" max="19" width="22.88671875" customWidth="1"/>
+    <col min="20" max="20" width="25.6640625" customWidth="1"/>
+    <col min="21" max="21" width="16.88671875" customWidth="1"/>
+    <col min="22" max="22" width="21.44140625" customWidth="1"/>
+    <col min="23" max="24" width="21.6640625" customWidth="1"/>
+    <col min="26" max="26" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -689,7 +722,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -769,7 +802,7 @@
         <v>0.84993812930119494</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -849,7 +882,7 @@
         <v>0.89712118945643604</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -929,7 +962,7 @@
         <v>0.91315153325116905</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1009,7 +1042,7 @@
         <v>0.88835512676806705</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -1089,7 +1122,7 @@
         <v>0.70690260888925904</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -1169,7 +1202,7 @@
         <v>0.92955667262784403</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1249,7 +1282,7 @@
         <v>0.93117267011921301</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1329,7 +1362,7 @@
         <v>0.915979846426349</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1409,7 +1442,7 @@
         <v>0.94089878006680805</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1489,7 +1522,7 @@
         <v>0.89968698888305798</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1569,7 +1602,7 @@
         <v>0.74096840257228003</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1649,7 +1682,7 @@
         <v>0.92621016479573504</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -1729,7 +1762,7 @@
         <v>0.88723255429597903</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1809,7 +1842,7 @@
         <v>0.94194838226724198</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1889,7 +1922,7 @@
         <v>0.91069366916296102</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -1969,7 +2002,7 @@
         <v>0.94141941148947805</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -2049,7 +2082,7 @@
         <v>0.87763498708068499</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -2129,7 +2162,7 @@
         <v>0.92921768872404498</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -2209,7 +2242,7 @@
         <v>0.89902900342229797</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -2289,7 +2322,7 @@
         <v>0.94322839017608295</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -2369,7 +2402,7 @@
         <v>0.94560638132603503</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -2449,7 +2482,7 @@
         <v>0.93739665152246499</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -2529,7 +2562,7 @@
         <v>0.92489003291190297</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -2609,7 +2642,7 @@
         <v>0.96102443963912498</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -2689,7 +2722,7 @@
         <v>0.87465768151022905</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -2769,7 +2802,7 @@
         <v>0.94245968994508</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -2849,7 +2882,7 @@
         <v>0.91256166503078395</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -2929,7 +2962,7 @@
         <v>0.978681810896601</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -3009,7 +3042,7 @@
         <v>0.81227002598557096</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -3089,7 +3122,7 @@
         <v>0.895603128852412</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -3169,7 +3202,7 @@
         <v>0.82896350578697398</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>28</v>
       </c>
@@ -3249,7 +3282,7 @@
         <v>0.90295330354992298</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>28</v>
       </c>
@@ -3329,7 +3362,7 @@
         <v>0.949066163651059</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>28</v>
       </c>
@@ -3409,7 +3442,7 @@
         <v>0.83166421141397995</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>28</v>
       </c>
@@ -3487,6 +3520,4027 @@
       </c>
       <c r="AA36">
         <v>0.82867501183857795</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35BFEDB7-6652-4B12-9C6C-38895C5B5484}">
+  <dimension ref="A1:AA50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Z29" sqref="Z29:AA50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.77734375" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="3" max="24" width="24.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>91500</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>0.179949234978449</v>
+      </c>
+      <c r="D2">
+        <v>4.6582485651425597E-3</v>
+      </c>
+      <c r="E2">
+        <v>1066.47019291986</v>
+      </c>
+      <c r="F2">
+        <v>25.536819338875699</v>
+      </c>
+      <c r="G2">
+        <v>1.86911596215967</v>
+      </c>
+      <c r="H2">
+        <v>4.9453958072034399E-2</v>
+      </c>
+      <c r="I2">
+        <v>1069.5298001036199</v>
+      </c>
+      <c r="J2">
+        <v>17.683016418376699</v>
+      </c>
+      <c r="K2">
+        <v>5.7263172325180897E-2</v>
+      </c>
+      <c r="L2">
+        <v>5.7389268607995004E-3</v>
+      </c>
+      <c r="M2">
+        <v>1124.3654618347</v>
+      </c>
+      <c r="N2">
+        <v>109.507628377511</v>
+      </c>
+      <c r="O2">
+        <v>7.5543727604257302E-2</v>
+      </c>
+      <c r="P2">
+        <v>1.04212748316426E-3</v>
+      </c>
+      <c r="Q2">
+        <v>1080.99412614675</v>
+      </c>
+      <c r="R2">
+        <v>27.521903374842001</v>
+      </c>
+      <c r="S2">
+        <v>5.5583303206811197</v>
+      </c>
+      <c r="T2">
+        <v>0.15147045401300899</v>
+      </c>
+      <c r="U2">
+        <v>2.82686145207694</v>
+      </c>
+      <c r="V2">
+        <v>77.459473395705501</v>
+      </c>
+      <c r="W2">
+        <v>27.835605605833301</v>
+      </c>
+      <c r="X2">
+        <v>14.944780298015299</v>
+      </c>
+      <c r="Z2">
+        <v>0.98455197189177601</v>
+      </c>
+      <c r="AA2">
+        <v>-0.26028609459894497</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>91500</v>
+      </c>
+      <c r="B3">
+        <v>101</v>
+      </c>
+      <c r="C3">
+        <v>0.17929333146618101</v>
+      </c>
+      <c r="D3">
+        <v>5.2933038854941104E-3</v>
+      </c>
+      <c r="E3">
+        <v>1062.8217566737001</v>
+      </c>
+      <c r="F3">
+        <v>28.854560597846699</v>
+      </c>
+      <c r="G3">
+        <v>1.84571420976491</v>
+      </c>
+      <c r="H3">
+        <v>5.5823528742289699E-2</v>
+      </c>
+      <c r="I3">
+        <v>1061.0405518100999</v>
+      </c>
+      <c r="J3">
+        <v>19.618373331677599</v>
+      </c>
+      <c r="K3">
+        <v>5.3480000781090602E-2</v>
+      </c>
+      <c r="L3">
+        <v>4.3739856382374398E-3</v>
+      </c>
+      <c r="M3">
+        <v>1052.4396968865899</v>
+      </c>
+      <c r="N3">
+        <v>83.784227173820398</v>
+      </c>
+      <c r="O3">
+        <v>7.4828523962281498E-2</v>
+      </c>
+      <c r="P3">
+        <v>1.1695509726695999E-3</v>
+      </c>
+      <c r="Q3">
+        <v>1061.5629298516101</v>
+      </c>
+      <c r="R3">
+        <v>31.312176659914002</v>
+      </c>
+      <c r="S3">
+        <v>5.5824533213638698</v>
+      </c>
+      <c r="T3">
+        <v>0.15994627565483199</v>
+      </c>
+      <c r="U3">
+        <v>2.6349825842359298</v>
+      </c>
+      <c r="V3">
+        <v>80.813697538323495</v>
+      </c>
+      <c r="W3">
+        <v>30.771237351274799</v>
+      </c>
+      <c r="X3">
+        <v>15.128405108268501</v>
+      </c>
+      <c r="Z3">
+        <v>0.95848649867817504</v>
+      </c>
+      <c r="AA3">
+        <v>1.70810040968386E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>91500</v>
+      </c>
+      <c r="B4">
+        <v>102</v>
+      </c>
+      <c r="C4">
+        <v>0.17783172920634699</v>
+      </c>
+      <c r="D4">
+        <v>5.0336803833617898E-3</v>
+      </c>
+      <c r="E4">
+        <v>1054.8547870396801</v>
+      </c>
+      <c r="F4">
+        <v>27.4430322731926</v>
+      </c>
+      <c r="G4">
+        <v>1.83147814271745</v>
+      </c>
+      <c r="H4">
+        <v>7.0912385952589405E-2</v>
+      </c>
+      <c r="I4">
+        <v>1055.35894467091</v>
+      </c>
+      <c r="J4">
+        <v>25.665296077173601</v>
+      </c>
+      <c r="K4">
+        <v>5.4086132372966202E-2</v>
+      </c>
+      <c r="L4">
+        <v>3.9389374151474798E-3</v>
+      </c>
+      <c r="M4">
+        <v>1064.2196248943501</v>
+      </c>
+      <c r="N4">
+        <v>75.246527945443404</v>
+      </c>
+      <c r="O4">
+        <v>7.4752486283262004E-2</v>
+      </c>
+      <c r="P4">
+        <v>1.84098972882089E-3</v>
+      </c>
+      <c r="Q4">
+        <v>1057.38023648697</v>
+      </c>
+      <c r="R4">
+        <v>49.5158835858023</v>
+      </c>
+      <c r="S4">
+        <v>5.6266354805749801</v>
+      </c>
+      <c r="T4">
+        <v>0.15297806504647599</v>
+      </c>
+      <c r="U4">
+        <v>2.6480980592071801</v>
+      </c>
+      <c r="V4">
+        <v>79.691645440644194</v>
+      </c>
+      <c r="W4">
+        <v>29.947890390721302</v>
+      </c>
+      <c r="X4">
+        <v>14.8740394480205</v>
+      </c>
+      <c r="Z4">
+        <v>0.96251051118264697</v>
+      </c>
+      <c r="AA4">
+        <v>8.9254891872986103E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>91500</v>
+      </c>
+      <c r="B5">
+        <v>103</v>
+      </c>
+      <c r="C5">
+        <v>0.180309458936256</v>
+      </c>
+      <c r="D5">
+        <v>6.2607549391361199E-3</v>
+      </c>
+      <c r="E5">
+        <v>1068.2608670712</v>
+      </c>
+      <c r="F5">
+        <v>33.944710661380597</v>
+      </c>
+      <c r="G5">
+        <v>1.8632880215274701</v>
+      </c>
+      <c r="H5">
+        <v>7.3095453377575101E-2</v>
+      </c>
+      <c r="I5">
+        <v>1066.6849145380199</v>
+      </c>
+      <c r="J5">
+        <v>25.657334221436599</v>
+      </c>
+      <c r="K5">
+        <v>5.2637229741586897E-2</v>
+      </c>
+      <c r="L5">
+        <v>3.3018678318770499E-3</v>
+      </c>
+      <c r="M5">
+        <v>1036.59443726688</v>
+      </c>
+      <c r="N5">
+        <v>63.354829866090697</v>
+      </c>
+      <c r="O5">
+        <v>7.4994182850457503E-2</v>
+      </c>
+      <c r="P5">
+        <v>1.5655655865073001E-3</v>
+      </c>
+      <c r="Q5">
+        <v>1064.8037433504201</v>
+      </c>
+      <c r="R5">
+        <v>42.917540390402102</v>
+      </c>
+      <c r="S5">
+        <v>5.5581051049855503</v>
+      </c>
+      <c r="T5">
+        <v>0.17780624189941699</v>
+      </c>
+      <c r="U5">
+        <v>2.59198439831105</v>
+      </c>
+      <c r="V5">
+        <v>81.805657596702403</v>
+      </c>
+      <c r="W5">
+        <v>31.6695289926942</v>
+      </c>
+      <c r="X5">
+        <v>15.074314371995101</v>
+      </c>
+      <c r="Z5">
+        <v>0.96138177756249998</v>
+      </c>
+      <c r="AA5">
+        <v>0.34189338920861301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>91500</v>
+      </c>
+      <c r="B6">
+        <v>104</v>
+      </c>
+      <c r="C6">
+        <v>0.18146533403012299</v>
+      </c>
+      <c r="D6">
+        <v>4.2908776518840999E-3</v>
+      </c>
+      <c r="E6">
+        <v>1074.7837010657099</v>
+      </c>
+      <c r="F6">
+        <v>23.398766102195601</v>
+      </c>
+      <c r="G6">
+        <v>1.8628008910883</v>
+      </c>
+      <c r="H6">
+        <v>4.3562812734607902E-2</v>
+      </c>
+      <c r="I6">
+        <v>1067.4522715655401</v>
+      </c>
+      <c r="J6">
+        <v>15.431755171973199</v>
+      </c>
+      <c r="K6">
+        <v>5.4759358672059201E-2</v>
+      </c>
+      <c r="L6">
+        <v>4.3580226607539E-3</v>
+      </c>
+      <c r="M6">
+        <v>1076.9879017531</v>
+      </c>
+      <c r="N6">
+        <v>83.264702062963195</v>
+      </c>
+      <c r="O6">
+        <v>7.4484032445990694E-2</v>
+      </c>
+      <c r="P6">
+        <v>1.2356731436885501E-3</v>
+      </c>
+      <c r="Q6">
+        <v>1052.0764254037599</v>
+      </c>
+      <c r="R6">
+        <v>33.4889770412641</v>
+      </c>
+      <c r="S6">
+        <v>5.5092507288470296</v>
+      </c>
+      <c r="T6">
+        <v>0.129760327369386</v>
+      </c>
+      <c r="U6">
+        <v>2.6396448278220799</v>
+      </c>
+      <c r="V6">
+        <v>81.185759282080596</v>
+      </c>
+      <c r="W6">
+        <v>30.7670321384192</v>
+      </c>
+      <c r="X6">
+        <v>14.999353174901</v>
+      </c>
+      <c r="Z6">
+        <v>0.97544385104133502</v>
+      </c>
+      <c r="AA6">
+        <v>-0.10777917554384001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>91500</v>
+      </c>
+      <c r="B7">
+        <v>105</v>
+      </c>
+      <c r="C7">
+        <v>0.177661391337295</v>
+      </c>
+      <c r="D7">
+        <v>4.3701893530796202E-3</v>
+      </c>
+      <c r="E7">
+        <v>1053.98586259323</v>
+      </c>
+      <c r="F7">
+        <v>23.956209057038901</v>
+      </c>
+      <c r="G7">
+        <v>1.8398162586239399</v>
+      </c>
+      <c r="H7">
+        <v>5.8966015541982997E-2</v>
+      </c>
+      <c r="I7">
+        <v>1058.8086282843601</v>
+      </c>
+      <c r="J7">
+        <v>21.111448428817202</v>
+      </c>
+      <c r="K7">
+        <v>5.4692654446174202E-2</v>
+      </c>
+      <c r="L7">
+        <v>4.4387340202446599E-3</v>
+      </c>
+      <c r="M7">
+        <v>1075.6804804139299</v>
+      </c>
+      <c r="N7">
+        <v>84.778922213867304</v>
+      </c>
+      <c r="O7">
+        <v>7.5028615056028702E-2</v>
+      </c>
+      <c r="P7">
+        <v>1.36901851050154E-3</v>
+      </c>
+      <c r="Q7">
+        <v>1066.3858291374099</v>
+      </c>
+      <c r="R7">
+        <v>36.9694250806523</v>
+      </c>
+      <c r="S7">
+        <v>5.6290423789197597</v>
+      </c>
+      <c r="T7">
+        <v>0.14157596288015301</v>
+      </c>
+      <c r="U7">
+        <v>2.70393444876315</v>
+      </c>
+      <c r="V7">
+        <v>80.723486059459503</v>
+      </c>
+      <c r="W7">
+        <v>29.975922712994102</v>
+      </c>
+      <c r="X7">
+        <v>14.948433678916899</v>
+      </c>
+      <c r="Z7">
+        <v>0.88581806600381297</v>
+      </c>
+      <c r="AA7">
+        <v>-0.108563649911121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>91500</v>
+      </c>
+      <c r="B8">
+        <v>106</v>
+      </c>
+      <c r="C8">
+        <v>0.17967039451574399</v>
+      </c>
+      <c r="D8">
+        <v>5.0749937993350598E-3</v>
+      </c>
+      <c r="E8">
+        <v>1064.90465851813</v>
+      </c>
+      <c r="F8">
+        <v>27.7805501774927</v>
+      </c>
+      <c r="G8">
+        <v>1.85741308368943</v>
+      </c>
+      <c r="H8">
+        <v>6.0501499431866702E-2</v>
+      </c>
+      <c r="I8">
+        <v>1065.0450270367901</v>
+      </c>
+      <c r="J8">
+        <v>21.475848293421901</v>
+      </c>
+      <c r="K8">
+        <v>5.5051142030230003E-2</v>
+      </c>
+      <c r="L8">
+        <v>5.1008003210662196E-3</v>
+      </c>
+      <c r="M8">
+        <v>1082.29351908544</v>
+      </c>
+      <c r="N8">
+        <v>97.559885624791207</v>
+      </c>
+      <c r="O8">
+        <v>7.4854550220297897E-2</v>
+      </c>
+      <c r="P8">
+        <v>1.04463877343841E-3</v>
+      </c>
+      <c r="Q8">
+        <v>1062.5566599250301</v>
+      </c>
+      <c r="R8">
+        <v>27.885621676548801</v>
+      </c>
+      <c r="S8">
+        <v>5.5714004344425199</v>
+      </c>
+      <c r="T8">
+        <v>0.16164729699282701</v>
+      </c>
+      <c r="U8">
+        <v>2.6834264463578199</v>
+      </c>
+      <c r="V8">
+        <v>79.483735635730199</v>
+      </c>
+      <c r="W8">
+        <v>30.017183281325298</v>
+      </c>
+      <c r="X8">
+        <v>15.059940294918</v>
+      </c>
+      <c r="Z8">
+        <v>0.83987037617675997</v>
+      </c>
+      <c r="AA8">
+        <v>0.33001411638341099</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>91500</v>
+      </c>
+      <c r="B9">
+        <v>107</v>
+      </c>
+      <c r="C9">
+        <v>0.17680197244620999</v>
+      </c>
+      <c r="D9">
+        <v>4.18184882438316E-3</v>
+      </c>
+      <c r="E9">
+        <v>1049.29635286959</v>
+      </c>
+      <c r="F9">
+        <v>22.942445666132699</v>
+      </c>
+      <c r="G9">
+        <v>1.83736650417748</v>
+      </c>
+      <c r="H9">
+        <v>4.5332877708895998E-2</v>
+      </c>
+      <c r="I9">
+        <v>1058.3265090104801</v>
+      </c>
+      <c r="J9">
+        <v>16.4188218960815</v>
+      </c>
+      <c r="K9">
+        <v>5.35804436438099E-2</v>
+      </c>
+      <c r="L9">
+        <v>3.2094712086351402E-3</v>
+      </c>
+      <c r="M9">
+        <v>1054.7284964733301</v>
+      </c>
+      <c r="N9">
+        <v>61.482132338589402</v>
+      </c>
+      <c r="O9">
+        <v>7.5212716422770207E-2</v>
+      </c>
+      <c r="P9">
+        <v>6.9442918009416602E-4</v>
+      </c>
+      <c r="Q9">
+        <v>1072.7868966814999</v>
+      </c>
+      <c r="R9">
+        <v>18.556862011340499</v>
+      </c>
+      <c r="S9">
+        <v>5.6558187454897801</v>
+      </c>
+      <c r="T9">
+        <v>0.13770218258797301</v>
+      </c>
+      <c r="U9">
+        <v>2.68524291806711</v>
+      </c>
+      <c r="V9">
+        <v>78.418496618622001</v>
+      </c>
+      <c r="W9">
+        <v>29.232754703673699</v>
+      </c>
+      <c r="X9">
+        <v>14.8437450786044</v>
+      </c>
+      <c r="Z9">
+        <v>0.95272526405569602</v>
+      </c>
+      <c r="AA9">
+        <v>-0.12380181298757199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>91500</v>
+      </c>
+      <c r="B10">
+        <v>108</v>
+      </c>
+      <c r="C10">
+        <v>0.180057063635984</v>
+      </c>
+      <c r="D10">
+        <v>4.5513279670111404E-3</v>
+      </c>
+      <c r="E10">
+        <v>1067.0715125592999</v>
+      </c>
+      <c r="F10">
+        <v>24.7840178057196</v>
+      </c>
+      <c r="G10">
+        <v>1.84803880682771</v>
+      </c>
+      <c r="H10">
+        <v>5.2140912962580901E-2</v>
+      </c>
+      <c r="I10">
+        <v>1061.96868097984</v>
+      </c>
+      <c r="J10">
+        <v>18.5278498009103</v>
+      </c>
+      <c r="K10">
+        <v>5.2566287611628799E-2</v>
+      </c>
+      <c r="L10">
+        <v>3.76453135372348E-3</v>
+      </c>
+      <c r="M10">
+        <v>1035.09706796557</v>
+      </c>
+      <c r="N10">
+        <v>72.196896295400606</v>
+      </c>
+      <c r="O10">
+        <v>7.4287112647192302E-2</v>
+      </c>
+      <c r="P10">
+        <v>1.7052155810837299E-3</v>
+      </c>
+      <c r="Q10">
+        <v>1045.25492853997</v>
+      </c>
+      <c r="R10">
+        <v>46.305666021514199</v>
+      </c>
+      <c r="S10">
+        <v>5.5548627938209103</v>
+      </c>
+      <c r="T10">
+        <v>0.13532187446890001</v>
+      </c>
+      <c r="U10">
+        <v>2.5714424553172699</v>
+      </c>
+      <c r="V10">
+        <v>80.209794334746405</v>
+      </c>
+      <c r="W10">
+        <v>31.402689151510899</v>
+      </c>
+      <c r="X10">
+        <v>15.122155887157399</v>
+      </c>
+      <c r="Z10">
+        <v>0.89616407851246804</v>
+      </c>
+      <c r="AA10">
+        <v>9.1164414864858406E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>91500</v>
+      </c>
+      <c r="B11">
+        <v>109</v>
+      </c>
+      <c r="C11">
+        <v>0.17965476176978201</v>
+      </c>
+      <c r="D11">
+        <v>4.2738595179908304E-3</v>
+      </c>
+      <c r="E11">
+        <v>1064.89899871324</v>
+      </c>
+      <c r="F11">
+        <v>23.254612772643998</v>
+      </c>
+      <c r="G11">
+        <v>1.84560264752837</v>
+      </c>
+      <c r="H11">
+        <v>5.2901198082762398E-2</v>
+      </c>
+      <c r="I11">
+        <v>1061.0665862999299</v>
+      </c>
+      <c r="J11">
+        <v>18.985519859260801</v>
+      </c>
+      <c r="K11">
+        <v>5.3471157286652103E-2</v>
+      </c>
+      <c r="L11">
+        <v>4.3815032999253399E-3</v>
+      </c>
+      <c r="M11">
+        <v>1052.2677828296401</v>
+      </c>
+      <c r="N11">
+        <v>83.865897696933004</v>
+      </c>
+      <c r="O11">
+        <v>7.42491869321147E-2</v>
+      </c>
+      <c r="P11">
+        <v>1.2775474718817799E-3</v>
+      </c>
+      <c r="Q11">
+        <v>1045.5738472181199</v>
+      </c>
+      <c r="R11">
+        <v>34.9632995455638</v>
+      </c>
+      <c r="S11">
+        <v>5.5656077815623304</v>
+      </c>
+      <c r="T11">
+        <v>0.125855308670376</v>
+      </c>
+      <c r="U11">
+        <v>2.71515958026096</v>
+      </c>
+      <c r="V11">
+        <v>80.644408420321298</v>
+      </c>
+      <c r="W11">
+        <v>30.1768605328818</v>
+      </c>
+      <c r="X11">
+        <v>14.972476382801201</v>
+      </c>
+      <c r="Z11">
+        <v>0.92589546011165202</v>
+      </c>
+      <c r="AA11">
+        <v>-0.25426156565444402</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>91500</v>
+      </c>
+      <c r="B12">
+        <v>110</v>
+      </c>
+      <c r="C12">
+        <v>0.18014782525214201</v>
+      </c>
+      <c r="D12">
+        <v>6.1393915309141001E-3</v>
+      </c>
+      <c r="E12">
+        <v>1067.3904551943999</v>
+      </c>
+      <c r="F12">
+        <v>33.482092229866097</v>
+      </c>
+      <c r="G12">
+        <v>1.86835054307836</v>
+      </c>
+      <c r="H12">
+        <v>8.0505836541551995E-2</v>
+      </c>
+      <c r="I12">
+        <v>1068.1692622542701</v>
+      </c>
+      <c r="J12">
+        <v>28.2403834744606</v>
+      </c>
+      <c r="K12">
+        <v>5.5155867195370703E-2</v>
+      </c>
+      <c r="L12">
+        <v>4.62045650410028E-3</v>
+      </c>
+      <c r="M12">
+        <v>1084.4910926540499</v>
+      </c>
+      <c r="N12">
+        <v>88.352624927987904</v>
+      </c>
+      <c r="O12">
+        <v>7.4854611475445906E-2</v>
+      </c>
+      <c r="P12">
+        <v>1.11095831816055E-3</v>
+      </c>
+      <c r="Q12">
+        <v>1062.4001388412901</v>
+      </c>
+      <c r="R12">
+        <v>29.819543407532901</v>
+      </c>
+      <c r="S12">
+        <v>5.5656983682307599</v>
+      </c>
+      <c r="T12">
+        <v>0.187000922803332</v>
+      </c>
+      <c r="U12">
+        <v>2.8294909126509298</v>
+      </c>
+      <c r="V12">
+        <v>78.945500460951294</v>
+      </c>
+      <c r="W12">
+        <v>28.5926023830053</v>
+      </c>
+      <c r="X12">
+        <v>15.005791312467499</v>
+      </c>
+      <c r="Z12">
+        <v>0.92341517650981897</v>
+      </c>
+      <c r="AA12">
+        <v>3.3903549011447098E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>91500</v>
+      </c>
+      <c r="B13">
+        <v>96</v>
+      </c>
+      <c r="C13">
+        <v>0.180509328527972</v>
+      </c>
+      <c r="D13">
+        <v>5.4802974437642002E-3</v>
+      </c>
+      <c r="E13">
+        <v>1069.4454418289299</v>
+      </c>
+      <c r="F13">
+        <v>29.818059536243702</v>
+      </c>
+      <c r="G13">
+        <v>1.86221436529512</v>
+      </c>
+      <c r="H13">
+        <v>6.5371694640384906E-2</v>
+      </c>
+      <c r="I13">
+        <v>1066.57047637142</v>
+      </c>
+      <c r="J13">
+        <v>23.342233901584901</v>
+      </c>
+      <c r="K13">
+        <v>5.2699794476931003E-2</v>
+      </c>
+      <c r="L13">
+        <v>4.2016455684123401E-3</v>
+      </c>
+      <c r="M13">
+        <v>1037.5181635569099</v>
+      </c>
+      <c r="N13">
+        <v>80.664719570978804</v>
+      </c>
+      <c r="O13">
+        <v>7.5187609830039498E-2</v>
+      </c>
+      <c r="P13">
+        <v>1.2400502260210399E-3</v>
+      </c>
+      <c r="Q13">
+        <v>1070.98728261512</v>
+      </c>
+      <c r="R13">
+        <v>33.657988340682401</v>
+      </c>
+      <c r="S13">
+        <v>5.5445824186147998</v>
+      </c>
+      <c r="T13">
+        <v>0.16226983751877899</v>
+      </c>
+      <c r="U13">
+        <v>2.5778692778910601</v>
+      </c>
+      <c r="V13">
+        <v>78.884184369151896</v>
+      </c>
+      <c r="W13">
+        <v>30.790189299456198</v>
+      </c>
+      <c r="X13">
+        <v>14.9670508609127</v>
+      </c>
+      <c r="Z13">
+        <v>0.98615260276985495</v>
+      </c>
+      <c r="AA13">
+        <v>-0.26701018932053899</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>91500</v>
+      </c>
+      <c r="B14">
+        <v>97</v>
+      </c>
+      <c r="C14">
+        <v>0.180126737790194</v>
+      </c>
+      <c r="D14">
+        <v>5.2259265892817004E-3</v>
+      </c>
+      <c r="E14">
+        <v>1067.38352803574</v>
+      </c>
+      <c r="F14">
+        <v>28.472099962198001</v>
+      </c>
+      <c r="G14">
+        <v>1.8334454146775701</v>
+      </c>
+      <c r="H14">
+        <v>6.8437853850144101E-2</v>
+      </c>
+      <c r="I14">
+        <v>1056.18941370683</v>
+      </c>
+      <c r="J14">
+        <v>24.425026350672201</v>
+      </c>
+      <c r="K14">
+        <v>5.5548844225552702E-2</v>
+      </c>
+      <c r="L14">
+        <v>4.2842088932216801E-3</v>
+      </c>
+      <c r="M14">
+        <v>1092.1421018728699</v>
+      </c>
+      <c r="N14">
+        <v>81.951047342041306</v>
+      </c>
+      <c r="O14">
+        <v>7.4097107573870793E-2</v>
+      </c>
+      <c r="P14">
+        <v>1.19195209611537E-3</v>
+      </c>
+      <c r="Q14">
+        <v>1041.6907868476901</v>
+      </c>
+      <c r="R14">
+        <v>32.1834023840618</v>
+      </c>
+      <c r="S14">
+        <v>5.5549349969822597</v>
+      </c>
+      <c r="T14">
+        <v>0.157151720287031</v>
+      </c>
+      <c r="U14">
+        <v>2.78304608896604</v>
+      </c>
+      <c r="V14">
+        <v>81.621615376382096</v>
+      </c>
+      <c r="W14">
+        <v>29.4432537697414</v>
+      </c>
+      <c r="X14">
+        <v>15.0893681107717</v>
+      </c>
+      <c r="Z14">
+        <v>0.87386910702748599</v>
+      </c>
+      <c r="AA14">
+        <v>-0.26936268415922898</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>91500</v>
+      </c>
+      <c r="B15">
+        <v>98</v>
+      </c>
+      <c r="C15">
+        <v>0.177459435720728</v>
+      </c>
+      <c r="D15">
+        <v>4.8188547789696397E-3</v>
+      </c>
+      <c r="E15">
+        <v>1052.8374977784999</v>
+      </c>
+      <c r="F15">
+        <v>26.3796044434329</v>
+      </c>
+      <c r="G15">
+        <v>1.8316735118842999</v>
+      </c>
+      <c r="H15">
+        <v>5.7833896681514299E-2</v>
+      </c>
+      <c r="I15">
+        <v>1055.93038476119</v>
+      </c>
+      <c r="J15">
+        <v>20.6790670771985</v>
+      </c>
+      <c r="K15">
+        <v>5.3795011973318298E-2</v>
+      </c>
+      <c r="L15">
+        <v>5.1038115798734398E-3</v>
+      </c>
+      <c r="M15">
+        <v>1058.2009878870999</v>
+      </c>
+      <c r="N15">
+        <v>97.864578982893605</v>
+      </c>
+      <c r="O15">
+        <v>7.4750430519271702E-2</v>
+      </c>
+      <c r="P15">
+        <v>6.8850001117802095E-4</v>
+      </c>
+      <c r="Q15">
+        <v>1060.3961027591199</v>
+      </c>
+      <c r="R15">
+        <v>18.511099722616098</v>
+      </c>
+      <c r="S15">
+        <v>5.6366868077157601</v>
+      </c>
+      <c r="T15">
+        <v>0.15385399718468401</v>
+      </c>
+      <c r="U15">
+        <v>2.7370081855975998</v>
+      </c>
+      <c r="V15">
+        <v>79.827403148838101</v>
+      </c>
+      <c r="W15">
+        <v>29.438582079964501</v>
+      </c>
+      <c r="X15">
+        <v>14.936162011766401</v>
+      </c>
+      <c r="Z15">
+        <v>0.89219907163568202</v>
+      </c>
+      <c r="AA15">
+        <v>-0.30992496720958901</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>91500</v>
+      </c>
+      <c r="B16">
+        <v>99</v>
+      </c>
+      <c r="C16">
+        <v>0.178499454726437</v>
+      </c>
+      <c r="D16">
+        <v>3.7560813721720099E-3</v>
+      </c>
+      <c r="E16">
+        <v>1058.62449578633</v>
+      </c>
+      <c r="F16">
+        <v>20.546049039648</v>
+      </c>
+      <c r="G16">
+        <v>1.8496057118023801</v>
+      </c>
+      <c r="H16">
+        <v>5.3252195153510297E-2</v>
+      </c>
+      <c r="I16">
+        <v>1062.48704117579</v>
+      </c>
+      <c r="J16">
+        <v>19.058930951413299</v>
+      </c>
+      <c r="K16">
+        <v>5.21338809999276E-2</v>
+      </c>
+      <c r="L16">
+        <v>4.0106332293438299E-3</v>
+      </c>
+      <c r="M16">
+        <v>1026.70998626409</v>
+      </c>
+      <c r="N16">
+        <v>76.979421686641302</v>
+      </c>
+      <c r="O16">
+        <v>7.5412343838540202E-2</v>
+      </c>
+      <c r="P16">
+        <v>1.7885427385241699E-3</v>
+      </c>
+      <c r="Q16">
+        <v>1075.3023094774301</v>
+      </c>
+      <c r="R16">
+        <v>47.693340927090397</v>
+      </c>
+      <c r="S16">
+        <v>5.5966513687029602</v>
+      </c>
+      <c r="T16">
+        <v>0.11838486892800799</v>
+      </c>
+      <c r="U16">
+        <v>2.6417821997996702</v>
+      </c>
+      <c r="V16">
+        <v>79.286630473551796</v>
+      </c>
+      <c r="W16">
+        <v>30.033753103109401</v>
+      </c>
+      <c r="X16">
+        <v>15.017967673932899</v>
+      </c>
+      <c r="Z16">
+        <v>0.97774790937974199</v>
+      </c>
+      <c r="AA16">
+        <v>-4.0030256611553398E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17">
+        <v>36</v>
+      </c>
+      <c r="C17">
+        <v>9.7835356718248306E-2</v>
+      </c>
+      <c r="D17">
+        <v>2.42076288507508E-3</v>
+      </c>
+      <c r="E17">
+        <v>601.64030546596496</v>
+      </c>
+      <c r="F17">
+        <v>14.2060354946017</v>
+      </c>
+      <c r="G17">
+        <v>0.81071590169900098</v>
+      </c>
+      <c r="H17">
+        <v>1.9313803485675098E-2</v>
+      </c>
+      <c r="I17">
+        <v>602.59582661700199</v>
+      </c>
+      <c r="J17">
+        <v>10.824810521374999</v>
+      </c>
+      <c r="K17">
+        <v>3.42706282811178E-2</v>
+      </c>
+      <c r="L17">
+        <v>6.7455748172377799E-3</v>
+      </c>
+      <c r="M17">
+        <v>679.26173325877903</v>
+      </c>
+      <c r="N17">
+        <v>130.19849045640601</v>
+      </c>
+      <c r="O17">
+        <v>6.0432802884085403E-2</v>
+      </c>
+      <c r="P17">
+        <v>8.2774231986190597E-4</v>
+      </c>
+      <c r="Q17">
+        <v>616.89442438746505</v>
+      </c>
+      <c r="R17">
+        <v>29.606348289876799</v>
+      </c>
+      <c r="S17">
+        <v>10.2170782611364</v>
+      </c>
+      <c r="T17">
+        <v>0.25083803948920802</v>
+      </c>
+      <c r="U17">
+        <v>29.769161858446999</v>
+      </c>
+      <c r="V17">
+        <v>293.73904163124399</v>
+      </c>
+      <c r="W17">
+        <v>10.3350291494093</v>
+      </c>
+      <c r="X17">
+        <v>3.1278765531445401</v>
+      </c>
+      <c r="Z17">
+        <v>0.76212395536585398</v>
+      </c>
+      <c r="AA17">
+        <v>4.5711493687099099E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18">
+        <v>37</v>
+      </c>
+      <c r="C18">
+        <v>9.8214748022763504E-2</v>
+      </c>
+      <c r="D18">
+        <v>2.1913265166893302E-3</v>
+      </c>
+      <c r="E18">
+        <v>603.880421317946</v>
+      </c>
+      <c r="F18">
+        <v>12.859070522721201</v>
+      </c>
+      <c r="G18">
+        <v>0.81251162520139597</v>
+      </c>
+      <c r="H18">
+        <v>1.6515659088002399E-2</v>
+      </c>
+      <c r="I18">
+        <v>603.67236176862502</v>
+      </c>
+      <c r="J18">
+        <v>9.2517973154208892</v>
+      </c>
+      <c r="K18">
+        <v>3.9643811033240099E-2</v>
+      </c>
+      <c r="L18">
+        <v>9.7489761544440404E-3</v>
+      </c>
+      <c r="M18">
+        <v>782.01727010414197</v>
+      </c>
+      <c r="N18">
+        <v>186.42258250942501</v>
+      </c>
+      <c r="O18">
+        <v>6.0207543384147098E-2</v>
+      </c>
+      <c r="P18">
+        <v>6.0169922185709099E-4</v>
+      </c>
+      <c r="Q18">
+        <v>609.40841940506596</v>
+      </c>
+      <c r="R18">
+        <v>21.598061356365701</v>
+      </c>
+      <c r="S18">
+        <v>10.173968235439499</v>
+      </c>
+      <c r="T18">
+        <v>0.22637561005492099</v>
+      </c>
+      <c r="U18">
+        <v>34.650064550769898</v>
+      </c>
+      <c r="V18">
+        <v>287.54264254943803</v>
+      </c>
+      <c r="W18">
+        <v>9.6145834073575394</v>
+      </c>
+      <c r="X18">
+        <v>3.24030945449242</v>
+      </c>
+      <c r="Z18">
+        <v>0.98431883483021498</v>
+      </c>
+      <c r="AA18">
+        <v>-0.49697853454902002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19">
+        <v>38</v>
+      </c>
+      <c r="C19">
+        <v>9.8020782500004705E-2</v>
+      </c>
+      <c r="D19">
+        <v>1.62098181450267E-3</v>
+      </c>
+      <c r="E19">
+        <v>602.76790585771596</v>
+      </c>
+      <c r="F19">
+        <v>9.5101129115082799</v>
+      </c>
+      <c r="G19">
+        <v>0.81821483704725495</v>
+      </c>
+      <c r="H19">
+        <v>1.17732634106872E-2</v>
+      </c>
+      <c r="I19">
+        <v>606.95628473714203</v>
+      </c>
+      <c r="J19">
+        <v>6.5710223717269898</v>
+      </c>
+      <c r="K19">
+        <v>3.1574005169854202E-2</v>
+      </c>
+      <c r="L19">
+        <v>3.4862207768634398E-3</v>
+      </c>
+      <c r="M19">
+        <v>627.86261189628999</v>
+      </c>
+      <c r="N19">
+        <v>68.335276713225099</v>
+      </c>
+      <c r="O19">
+        <v>6.0637851450068003E-2</v>
+      </c>
+      <c r="P19">
+        <v>7.9573196193716798E-4</v>
+      </c>
+      <c r="Q19">
+        <v>624.29280389571295</v>
+      </c>
+      <c r="R19">
+        <v>28.579586781278699</v>
+      </c>
+      <c r="S19">
+        <v>10.1851582588917</v>
+      </c>
+      <c r="T19">
+        <v>0.16632063704830899</v>
+      </c>
+      <c r="U19">
+        <v>25.770602672470901</v>
+      </c>
+      <c r="V19">
+        <v>282.900520280975</v>
+      </c>
+      <c r="W19">
+        <v>11.0585917682402</v>
+      </c>
+      <c r="X19">
+        <v>3.1660799382198599</v>
+      </c>
+      <c r="Z19">
+        <v>0.96517273010348303</v>
+      </c>
+      <c r="AA19">
+        <v>2.20437587227954E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20">
+        <v>39</v>
+      </c>
+      <c r="C20">
+        <v>9.7902970068601006E-2</v>
+      </c>
+      <c r="D20">
+        <v>2.5837239414867302E-3</v>
+      </c>
+      <c r="E20">
+        <v>602.02755785259797</v>
+      </c>
+      <c r="F20">
+        <v>15.155691740809001</v>
+      </c>
+      <c r="G20">
+        <v>0.81293618450736504</v>
+      </c>
+      <c r="H20">
+        <v>2.2448108015307298E-2</v>
+      </c>
+      <c r="I20">
+        <v>603.75397743278802</v>
+      </c>
+      <c r="J20">
+        <v>12.4546803576111</v>
+      </c>
+      <c r="K20">
+        <v>5.4571210333111901E-2</v>
+      </c>
+      <c r="L20">
+        <v>3.5647277757890602E-2</v>
+      </c>
+      <c r="M20">
+        <v>1028.9569148631199</v>
+      </c>
+      <c r="N20">
+        <v>616.635016016382</v>
+      </c>
+      <c r="O20">
+        <v>6.0179880632793697E-2</v>
+      </c>
+      <c r="P20">
+        <v>7.0481961650703995E-4</v>
+      </c>
+      <c r="Q20">
+        <v>608.16680445154304</v>
+      </c>
+      <c r="R20">
+        <v>25.3405510657722</v>
+      </c>
+      <c r="S20">
+        <v>10.2178984419581</v>
+      </c>
+      <c r="T20">
+        <v>0.26514644818067001</v>
+      </c>
+      <c r="U20">
+        <v>45.063060576980099</v>
+      </c>
+      <c r="V20">
+        <v>282.41015259031701</v>
+      </c>
+      <c r="W20">
+        <v>10.0746074711834</v>
+      </c>
+      <c r="X20">
+        <v>3.1004637456260902</v>
+      </c>
+      <c r="Z20">
+        <v>0.94606012754874902</v>
+      </c>
+      <c r="AA20">
+        <v>9.1012584167616695E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21">
+        <v>40</v>
+      </c>
+      <c r="C21">
+        <v>9.7976810897138097E-2</v>
+      </c>
+      <c r="D21">
+        <v>1.4904737715415799E-3</v>
+      </c>
+      <c r="E21">
+        <v>602.51314174235301</v>
+      </c>
+      <c r="F21">
+        <v>8.74463617424286</v>
+      </c>
+      <c r="G21">
+        <v>0.80745150551920497</v>
+      </c>
+      <c r="H21">
+        <v>1.8320712426819399E-2</v>
+      </c>
+      <c r="I21">
+        <v>600.78027247816794</v>
+      </c>
+      <c r="J21">
+        <v>10.1461699698673</v>
+      </c>
+      <c r="K21">
+        <v>3.9595017140400798E-2</v>
+      </c>
+      <c r="L21">
+        <v>1.38388148959978E-2</v>
+      </c>
+      <c r="M21">
+        <v>776.79405218029694</v>
+      </c>
+      <c r="N21">
+        <v>261.23473550032998</v>
+      </c>
+      <c r="O21">
+        <v>5.9587304351289498E-2</v>
+      </c>
+      <c r="P21">
+        <v>8.5903107415950103E-4</v>
+      </c>
+      <c r="Q21">
+        <v>586.21251188308997</v>
+      </c>
+      <c r="R21">
+        <v>30.800322766800601</v>
+      </c>
+      <c r="S21">
+        <v>10.191297794499</v>
+      </c>
+      <c r="T21">
+        <v>0.15319532854444301</v>
+      </c>
+      <c r="U21">
+        <v>29.418991307908701</v>
+      </c>
+      <c r="V21">
+        <v>281.21948643133999</v>
+      </c>
+      <c r="W21">
+        <v>10.9374719915404</v>
+      </c>
+      <c r="X21">
+        <v>3.0387093643595402</v>
+      </c>
+      <c r="Z21">
+        <v>0.88860452852972305</v>
+      </c>
+      <c r="AA21">
+        <v>0.237126169605897</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22">
+        <v>41</v>
+      </c>
+      <c r="C22">
+        <v>9.7496129760535399E-2</v>
+      </c>
+      <c r="D22">
+        <v>2.1270760368424001E-3</v>
+      </c>
+      <c r="E22">
+        <v>599.66407432052199</v>
+      </c>
+      <c r="F22">
+        <v>12.4920933150169</v>
+      </c>
+      <c r="G22">
+        <v>0.816090321865938</v>
+      </c>
+      <c r="H22">
+        <v>1.9426678028688301E-2</v>
+      </c>
+      <c r="I22">
+        <v>605.60135778508698</v>
+      </c>
+      <c r="J22">
+        <v>10.9278638690742</v>
+      </c>
+      <c r="K22">
+        <v>3.8718228041039797E-2</v>
+      </c>
+      <c r="L22">
+        <v>1.24059199351463E-2</v>
+      </c>
+      <c r="M22">
+        <v>761.67861074950895</v>
+      </c>
+      <c r="N22">
+        <v>234.73190397585</v>
+      </c>
+      <c r="O22">
+        <v>6.0477039518480699E-2</v>
+      </c>
+      <c r="P22">
+        <v>5.7502105568471302E-4</v>
+      </c>
+      <c r="Q22">
+        <v>619.11658529594797</v>
+      </c>
+      <c r="R22">
+        <v>20.5574233965032</v>
+      </c>
+      <c r="S22">
+        <v>10.253065197707199</v>
+      </c>
+      <c r="T22">
+        <v>0.22408835324649501</v>
+      </c>
+      <c r="U22">
+        <v>35.054263543476999</v>
+      </c>
+      <c r="V22">
+        <v>287.53434872292598</v>
+      </c>
+      <c r="W22">
+        <v>10.2314624386114</v>
+      </c>
+      <c r="X22">
+        <v>3.0894823881417302</v>
+      </c>
+      <c r="Z22">
+        <v>0.99024766965492805</v>
+      </c>
+      <c r="AA22">
+        <v>0.24781017909206601</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23">
+        <v>21</v>
+      </c>
+      <c r="C23">
+        <v>8.5784663136933503E-2</v>
+      </c>
+      <c r="D23">
+        <v>2.5486389329664799E-3</v>
+      </c>
+      <c r="E23">
+        <v>530.479163711551</v>
+      </c>
+      <c r="F23">
+        <v>15.1118594976945</v>
+      </c>
+      <c r="G23">
+        <v>0.71093077956977302</v>
+      </c>
+      <c r="H23">
+        <v>3.2047242864864198E-2</v>
+      </c>
+      <c r="I23">
+        <v>544.52218277091299</v>
+      </c>
+      <c r="J23">
+        <v>18.577073703778101</v>
+      </c>
+      <c r="K23">
+        <v>3.1241993223163601E-2</v>
+      </c>
+      <c r="L23">
+        <v>1.53447626617084E-3</v>
+      </c>
+      <c r="M23">
+        <v>621.77259040070498</v>
+      </c>
+      <c r="N23">
+        <v>30.0800957624867</v>
+      </c>
+      <c r="O23">
+        <v>5.9445970203709897E-2</v>
+      </c>
+      <c r="P23">
+        <v>4.9833753508995201E-4</v>
+      </c>
+      <c r="Q23">
+        <v>582.02281688124197</v>
+      </c>
+      <c r="R23">
+        <v>18.192291053273799</v>
+      </c>
+      <c r="S23">
+        <v>11.519986739900601</v>
+      </c>
+      <c r="T23">
+        <v>0.437590726936742</v>
+      </c>
+      <c r="U23">
+        <v>1.2449827748104001</v>
+      </c>
+      <c r="V23">
+        <v>1017.07937037231</v>
+      </c>
+      <c r="W23">
+        <v>806.59261204526797</v>
+      </c>
+      <c r="X23">
+        <v>241.73857894535399</v>
+      </c>
+      <c r="Z23">
+        <v>0.81487491252676603</v>
+      </c>
+      <c r="AA23">
+        <v>-0.100657838800621</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24">
+        <v>22</v>
+      </c>
+      <c r="C24">
+        <v>8.6555746401771397E-2</v>
+      </c>
+      <c r="D24">
+        <v>2.7057368545348901E-3</v>
+      </c>
+      <c r="E24">
+        <v>535.04504064765194</v>
+      </c>
+      <c r="F24">
+        <v>16.064304634699599</v>
+      </c>
+      <c r="G24">
+        <v>0.70800070907268897</v>
+      </c>
+      <c r="H24">
+        <v>2.3213758111694599E-2</v>
+      </c>
+      <c r="I24">
+        <v>543.13635577372804</v>
+      </c>
+      <c r="J24">
+        <v>13.801538059985401</v>
+      </c>
+      <c r="K24">
+        <v>3.1335362834722401E-2</v>
+      </c>
+      <c r="L24">
+        <v>1.653828534666E-3</v>
+      </c>
+      <c r="M24">
+        <v>623.58662290194297</v>
+      </c>
+      <c r="N24">
+        <v>32.410307285234602</v>
+      </c>
+      <c r="O24">
+        <v>5.9634668216962103E-2</v>
+      </c>
+      <c r="P24">
+        <v>5.6210593293560803E-4</v>
+      </c>
+      <c r="Q24">
+        <v>588.77373745291004</v>
+      </c>
+      <c r="R24">
+        <v>20.551181000503501</v>
+      </c>
+      <c r="S24">
+        <v>11.5688116091211</v>
+      </c>
+      <c r="T24">
+        <v>0.36981196423684298</v>
+      </c>
+      <c r="U24">
+        <v>1.2647138700099101</v>
+      </c>
+      <c r="V24">
+        <v>1087.8686809906501</v>
+      </c>
+      <c r="W24">
+        <v>849.09151180112099</v>
+      </c>
+      <c r="X24">
+        <v>251.431054927471</v>
+      </c>
+      <c r="Z24">
+        <v>0.90410779463345903</v>
+      </c>
+      <c r="AA24">
+        <v>0.146657849612815</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25">
+        <v>23</v>
+      </c>
+      <c r="C25">
+        <v>8.7635311357749601E-2</v>
+      </c>
+      <c r="D25">
+        <v>3.5728465498406402E-3</v>
+      </c>
+      <c r="E25">
+        <v>541.38053006063103</v>
+      </c>
+      <c r="F25">
+        <v>21.154024742710401</v>
+      </c>
+      <c r="G25">
+        <v>0.71468620289311502</v>
+      </c>
+      <c r="H25">
+        <v>2.95839361417688E-2</v>
+      </c>
+      <c r="I25">
+        <v>546.85200033556498</v>
+      </c>
+      <c r="J25">
+        <v>17.3847479730969</v>
+      </c>
+      <c r="K25">
+        <v>3.0761529317290402E-2</v>
+      </c>
+      <c r="L25">
+        <v>1.72231706546692E-3</v>
+      </c>
+      <c r="M25">
+        <v>612.325009454108</v>
+      </c>
+      <c r="N25">
+        <v>33.772656230565701</v>
+      </c>
+      <c r="O25">
+        <v>5.9464137522014501E-2</v>
+      </c>
+      <c r="P25">
+        <v>6.3839056597865301E-4</v>
+      </c>
+      <c r="Q25">
+        <v>582.38728201887295</v>
+      </c>
+      <c r="R25">
+        <v>23.2807351631496</v>
+      </c>
+      <c r="S25">
+        <v>11.458952214779901</v>
+      </c>
+      <c r="T25">
+        <v>0.458733205738104</v>
+      </c>
+      <c r="U25">
+        <v>1.2408835577994899</v>
+      </c>
+      <c r="V25">
+        <v>1054.0101689528699</v>
+      </c>
+      <c r="W25">
+        <v>838.3512950132</v>
+      </c>
+      <c r="X25">
+        <v>243.27123653927299</v>
+      </c>
+      <c r="Z25">
+        <v>0.98379257150059396</v>
+      </c>
+      <c r="AA25">
+        <v>-0.32747731695779497</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26">
+        <v>24</v>
+      </c>
+      <c r="C26">
+        <v>8.7114166293273398E-2</v>
+      </c>
+      <c r="D26">
+        <v>2.8808328295137102E-3</v>
+      </c>
+      <c r="E26">
+        <v>538.33979840436405</v>
+      </c>
+      <c r="F26">
+        <v>17.076721935329999</v>
+      </c>
+      <c r="G26">
+        <v>0.71264887435330204</v>
+      </c>
+      <c r="H26">
+        <v>2.1835761182005298E-2</v>
+      </c>
+      <c r="I26">
+        <v>545.92415252221804</v>
+      </c>
+      <c r="J26">
+        <v>12.9902897349735</v>
+      </c>
+      <c r="K26">
+        <v>3.1168247877660999E-2</v>
+      </c>
+      <c r="L26">
+        <v>1.61429637526267E-3</v>
+      </c>
+      <c r="M26">
+        <v>620.31345542044301</v>
+      </c>
+      <c r="N26">
+        <v>31.664515109355499</v>
+      </c>
+      <c r="O26">
+        <v>5.9665657948752601E-2</v>
+      </c>
+      <c r="P26">
+        <v>5.6326782963101298E-4</v>
+      </c>
+      <c r="Q26">
+        <v>589.87129042392201</v>
+      </c>
+      <c r="R26">
+        <v>20.433020274749001</v>
+      </c>
+      <c r="S26">
+        <v>11.502484078437099</v>
+      </c>
+      <c r="T26">
+        <v>0.37864853005513099</v>
+      </c>
+      <c r="U26">
+        <v>1.2743427965137999</v>
+      </c>
+      <c r="V26">
+        <v>1078.53953757626</v>
+      </c>
+      <c r="W26">
+        <v>835.51250833926497</v>
+      </c>
+      <c r="X26">
+        <v>245.82880813082701</v>
+      </c>
+      <c r="Z26">
+        <v>0.96839759806252501</v>
+      </c>
+      <c r="AA26">
+        <v>0.123700406444559</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27">
+        <v>46</v>
+      </c>
+      <c r="C27">
+        <v>8.6979454132485604E-2</v>
+      </c>
+      <c r="D27">
+        <v>3.6731776095786902E-3</v>
+      </c>
+      <c r="E27">
+        <v>537.48299138973402</v>
+      </c>
+      <c r="F27">
+        <v>21.761195308438399</v>
+      </c>
+      <c r="G27">
+        <v>0.71440894711163305</v>
+      </c>
+      <c r="H27">
+        <v>3.3792198944965803E-2</v>
+      </c>
+      <c r="I27">
+        <v>546.47593851659303</v>
+      </c>
+      <c r="J27">
+        <v>19.972575280616699</v>
+      </c>
+      <c r="K27">
+        <v>3.0794145323293901E-2</v>
+      </c>
+      <c r="L27">
+        <v>1.7390573605928501E-3</v>
+      </c>
+      <c r="M27">
+        <v>612.96221948090397</v>
+      </c>
+      <c r="N27">
+        <v>34.0760086228671</v>
+      </c>
+      <c r="O27">
+        <v>5.9746927357421299E-2</v>
+      </c>
+      <c r="P27">
+        <v>7.1762836258890995E-4</v>
+      </c>
+      <c r="Q27">
+        <v>592.47589746936001</v>
+      </c>
+      <c r="R27">
+        <v>26.280773723695599</v>
+      </c>
+      <c r="S27">
+        <v>11.5530259955839</v>
+      </c>
+      <c r="T27">
+        <v>0.48103565648697399</v>
+      </c>
+      <c r="U27">
+        <v>1.2677028882882699</v>
+      </c>
+      <c r="V27">
+        <v>1077.965656868</v>
+      </c>
+      <c r="W27">
+        <v>839.45061628416602</v>
+      </c>
+      <c r="X27">
+        <v>251.067006461197</v>
+      </c>
+      <c r="Z27">
+        <v>0.96077147318062395</v>
+      </c>
+      <c r="AA27">
+        <v>-0.197668350666518</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28">
+        <v>47</v>
+      </c>
+      <c r="C28">
+        <v>8.7031722999962993E-2</v>
+      </c>
+      <c r="D28">
+        <v>2.9628333970996398E-3</v>
+      </c>
+      <c r="E28">
+        <v>537.85094723069506</v>
+      </c>
+      <c r="F28">
+        <v>17.529728545214699</v>
+      </c>
+      <c r="G28">
+        <v>0.71749594551161999</v>
+      </c>
+      <c r="H28">
+        <v>2.9490352706770001E-2</v>
+      </c>
+      <c r="I28">
+        <v>548.52831498406101</v>
+      </c>
+      <c r="J28">
+        <v>17.157680828184599</v>
+      </c>
+      <c r="K28">
+        <v>3.2512223408892697E-2</v>
+      </c>
+      <c r="L28">
+        <v>1.8213896227587301E-3</v>
+      </c>
+      <c r="M28">
+        <v>646.61818949990902</v>
+      </c>
+      <c r="N28">
+        <v>35.606496551067103</v>
+      </c>
+      <c r="O28">
+        <v>5.9729023361283398E-2</v>
+      </c>
+      <c r="P28">
+        <v>6.8700698303264898E-4</v>
+      </c>
+      <c r="Q28">
+        <v>591.91444929547299</v>
+      </c>
+      <c r="R28">
+        <v>24.9974865116342</v>
+      </c>
+      <c r="S28">
+        <v>11.5155120224226</v>
+      </c>
+      <c r="T28">
+        <v>0.37487660981978799</v>
+      </c>
+      <c r="U28">
+        <v>1.30582404399359</v>
+      </c>
+      <c r="V28">
+        <v>1060.18485372174</v>
+      </c>
+      <c r="W28">
+        <v>800.86012539243302</v>
+      </c>
+      <c r="X28">
+        <v>235.97675809661101</v>
+      </c>
+      <c r="Z28">
+        <v>0.85476973488241903</v>
+      </c>
+      <c r="AA28">
+        <v>0.34285658868267999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29">
+        <v>100</v>
+      </c>
+      <c r="C29">
+        <v>0.27505457767833003</v>
+      </c>
+      <c r="D29">
+        <v>1.0515876738305899E-2</v>
+      </c>
+      <c r="E29">
+        <v>1565.4215242421601</v>
+      </c>
+      <c r="F29">
+        <v>53.147965830935298</v>
+      </c>
+      <c r="G29">
+        <v>34.407652469604201</v>
+      </c>
+      <c r="H29">
+        <v>1.3766462728786799</v>
+      </c>
+      <c r="I29">
+        <v>3618.3499240686601</v>
+      </c>
+      <c r="J29">
+        <v>39.457272549061997</v>
+      </c>
+      <c r="K29">
+        <v>0.61106611930907895</v>
+      </c>
+      <c r="L29">
+        <v>5.36647220655928E-2</v>
+      </c>
+      <c r="M29">
+        <v>9599.1888275539404</v>
+      </c>
+      <c r="N29">
+        <v>671.77454296415397</v>
+      </c>
+      <c r="O29">
+        <v>0.90932855305132398</v>
+      </c>
+      <c r="P29">
+        <v>6.2442023340651201E-3</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>55</v>
+      </c>
+      <c r="R29" t="s">
+        <v>55</v>
+      </c>
+      <c r="S29">
+        <v>3.6489794499419599</v>
+      </c>
+      <c r="T29">
+        <v>0.140590624394338</v>
+      </c>
+      <c r="U29">
+        <v>0.98771212039017298</v>
+      </c>
+      <c r="V29">
+        <v>25.710856461124798</v>
+      </c>
+      <c r="W29">
+        <v>26.324672401216802</v>
+      </c>
+      <c r="X29">
+        <v>151.59325336094301</v>
+      </c>
+      <c r="Z29">
+        <v>0.93991777722373304</v>
+      </c>
+      <c r="AA29">
+        <v>0.285378114104748</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30">
+        <v>101</v>
+      </c>
+      <c r="C30">
+        <v>0.26762916057352099</v>
+      </c>
+      <c r="D30">
+        <v>1.0755512925962701E-2</v>
+      </c>
+      <c r="E30">
+        <v>1527.7009143528301</v>
+      </c>
+      <c r="F30">
+        <v>55.145988266321503</v>
+      </c>
+      <c r="G30">
+        <v>33.678397566135601</v>
+      </c>
+      <c r="H30">
+        <v>1.3349620730610099</v>
+      </c>
+      <c r="I30">
+        <v>3597.04484422308</v>
+      </c>
+      <c r="J30">
+        <v>41.146597174716398</v>
+      </c>
+      <c r="K30">
+        <v>0.59036703463207796</v>
+      </c>
+      <c r="L30">
+        <v>5.05629536988393E-2</v>
+      </c>
+      <c r="M30">
+        <v>9342.6727108862196</v>
+      </c>
+      <c r="N30">
+        <v>630.42562599052701</v>
+      </c>
+      <c r="O30">
+        <v>0.91460850493936696</v>
+      </c>
+      <c r="P30">
+        <v>9.4474262361090994E-3</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>55</v>
+      </c>
+      <c r="R30" t="s">
+        <v>55</v>
+      </c>
+      <c r="S30">
+        <v>3.75559310992969</v>
+      </c>
+      <c r="T30">
+        <v>0.16685337102498199</v>
+      </c>
+      <c r="U30">
+        <v>0.97062107950210597</v>
+      </c>
+      <c r="V30">
+        <v>25.996400809955901</v>
+      </c>
+      <c r="W30">
+        <v>27.199352183914399</v>
+      </c>
+      <c r="X30">
+        <v>146.568647791312</v>
+      </c>
+      <c r="Z30">
+        <v>0.98218325139192297</v>
+      </c>
+      <c r="AA30">
+        <v>-0.47159499951594303</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31">
+        <v>102</v>
+      </c>
+      <c r="C31">
+        <v>0.25661507176361198</v>
+      </c>
+      <c r="D31">
+        <v>1.0692783813163499E-2</v>
+      </c>
+      <c r="E31">
+        <v>1471.4566888926499</v>
+      </c>
+      <c r="F31">
+        <v>54.607723745177502</v>
+      </c>
+      <c r="G31">
+        <v>32.119188415781203</v>
+      </c>
+      <c r="H31">
+        <v>1.2199499934715501</v>
+      </c>
+      <c r="I31">
+        <v>3550.9018123593601</v>
+      </c>
+      <c r="J31">
+        <v>36.997581780838999</v>
+      </c>
+      <c r="K31">
+        <v>0.628092908642645</v>
+      </c>
+      <c r="L31">
+        <v>6.6671526116508506E-2</v>
+      </c>
+      <c r="M31">
+        <v>9788.1989819623504</v>
+      </c>
+      <c r="N31">
+        <v>808.20229149750901</v>
+      </c>
+      <c r="O31">
+        <v>0.90959058246422897</v>
+      </c>
+      <c r="P31">
+        <v>9.1491114009919407E-3</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>55</v>
+      </c>
+      <c r="R31" t="s">
+        <v>55</v>
+      </c>
+      <c r="S31">
+        <v>3.91523754297216</v>
+      </c>
+      <c r="T31">
+        <v>0.15809768601889501</v>
+      </c>
+      <c r="U31">
+        <v>1.0556281233250999</v>
+      </c>
+      <c r="V31">
+        <v>27.2080680291789</v>
+      </c>
+      <c r="W31">
+        <v>26.4037506830457</v>
+      </c>
+      <c r="X31">
+        <v>148.256549473224</v>
+      </c>
+      <c r="Z31">
+        <v>0.96246211677138804</v>
+      </c>
+      <c r="AA31">
+        <v>0.181141347980083</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32">
+        <v>103</v>
+      </c>
+      <c r="C32">
+        <v>0.26703949743151001</v>
+      </c>
+      <c r="D32">
+        <v>9.9136025908138498E-3</v>
+      </c>
+      <c r="E32">
+        <v>1524.8226366977301</v>
+      </c>
+      <c r="F32">
+        <v>50.3270694658152</v>
+      </c>
+      <c r="G32">
+        <v>33.224196536568002</v>
+      </c>
+      <c r="H32">
+        <v>1.15391089878639</v>
+      </c>
+      <c r="I32">
+        <v>3584.5812952787901</v>
+      </c>
+      <c r="J32">
+        <v>33.845495740776798</v>
+      </c>
+      <c r="K32">
+        <v>0.60140381878244398</v>
+      </c>
+      <c r="L32">
+        <v>5.8319264883086801E-2</v>
+      </c>
+      <c r="M32">
+        <v>9466.1956841792598</v>
+      </c>
+      <c r="N32">
+        <v>719.87379325563597</v>
+      </c>
+      <c r="O32">
+        <v>0.90326658368784396</v>
+      </c>
+      <c r="P32">
+        <v>7.1859044921330304E-3</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>55</v>
+      </c>
+      <c r="R32" t="s">
+        <v>55</v>
+      </c>
+      <c r="S32">
+        <v>3.7584654716193602</v>
+      </c>
+      <c r="T32">
+        <v>0.13801504042755999</v>
+      </c>
+      <c r="U32">
+        <v>0.96910163855600795</v>
+      </c>
+      <c r="V32">
+        <v>26.275962784301498</v>
+      </c>
+      <c r="W32">
+        <v>27.334626341792799</v>
+      </c>
+      <c r="X32">
+        <v>143.67484972071</v>
+      </c>
+      <c r="Z32">
+        <v>0.985074149783568</v>
+      </c>
+      <c r="AA32">
+        <v>5.8920597230304302E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33">
+        <v>104</v>
+      </c>
+      <c r="C33">
+        <v>0.25809301766638498</v>
+      </c>
+      <c r="D33">
+        <v>5.7504716484574597E-3</v>
+      </c>
+      <c r="E33">
+        <v>1479.77524805656</v>
+      </c>
+      <c r="F33">
+        <v>29.443721134194501</v>
+      </c>
+      <c r="G33">
+        <v>32.470507091716897</v>
+      </c>
+      <c r="H33">
+        <v>0.75657672454741698</v>
+      </c>
+      <c r="I33">
+        <v>3563.5165237526098</v>
+      </c>
+      <c r="J33">
+        <v>22.741695649238199</v>
+      </c>
+      <c r="K33">
+        <v>0.58788274846088895</v>
+      </c>
+      <c r="L33">
+        <v>4.38237386868644E-2</v>
+      </c>
+      <c r="M33">
+        <v>9321.0918538260794</v>
+      </c>
+      <c r="N33">
+        <v>563.49025561901703</v>
+      </c>
+      <c r="O33">
+        <v>0.91231201315055799</v>
+      </c>
+      <c r="P33">
+        <v>6.1108117163363304E-3</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>55</v>
+      </c>
+      <c r="R33" t="s">
+        <v>55</v>
+      </c>
+      <c r="S33">
+        <v>3.8724601535822298</v>
+      </c>
+      <c r="T33">
+        <v>8.5985537297306805E-2</v>
+      </c>
+      <c r="U33">
+        <v>0.99257979528157003</v>
+      </c>
+      <c r="V33">
+        <v>27.143607328023698</v>
+      </c>
+      <c r="W33">
+        <v>27.3804782561424</v>
+      </c>
+      <c r="X33">
+        <v>142.93208428962899</v>
+      </c>
+      <c r="Z33">
+        <v>0.98077302429481805</v>
+      </c>
+      <c r="AA33">
+        <v>-0.48480509703833902</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34">
+        <v>105</v>
+      </c>
+      <c r="C34">
+        <v>0.261503262121144</v>
+      </c>
+      <c r="D34">
+        <v>1.32780060149648E-2</v>
+      </c>
+      <c r="E34">
+        <v>1495.8291294222699</v>
+      </c>
+      <c r="F34">
+        <v>67.943786825578599</v>
+      </c>
+      <c r="G34">
+        <v>32.863671814252399</v>
+      </c>
+      <c r="H34">
+        <v>1.6136617970878999</v>
+      </c>
+      <c r="I34">
+        <v>3570.9158034350298</v>
+      </c>
+      <c r="J34">
+        <v>49.3132395308713</v>
+      </c>
+      <c r="K34">
+        <v>0.56766967696399895</v>
+      </c>
+      <c r="L34">
+        <v>5.4676078360437599E-2</v>
+      </c>
+      <c r="M34">
+        <v>9040.2606249767396</v>
+      </c>
+      <c r="N34">
+        <v>689.37546815566998</v>
+      </c>
+      <c r="O34">
+        <v>0.91111347435738599</v>
+      </c>
+      <c r="P34">
+        <v>6.5139665002670903E-3</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>55</v>
+      </c>
+      <c r="R34" t="s">
+        <v>55</v>
+      </c>
+      <c r="S34">
+        <v>3.86215168214913</v>
+      </c>
+      <c r="T34">
+        <v>0.20290794312857599</v>
+      </c>
+      <c r="U34">
+        <v>0.96236887294805895</v>
+      </c>
+      <c r="V34">
+        <v>26.8641359771648</v>
+      </c>
+      <c r="W34">
+        <v>28.570942555077899</v>
+      </c>
+      <c r="X34">
+        <v>145.35689440468599</v>
+      </c>
+      <c r="Z34">
+        <v>0.91566399022467904</v>
+      </c>
+      <c r="AA34">
+        <v>0.43051660026260502</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35">
+        <v>106</v>
+      </c>
+      <c r="C35">
+        <v>0.26250465118689498</v>
+      </c>
+      <c r="D35">
+        <v>1.1479251446107E-2</v>
+      </c>
+      <c r="E35">
+        <v>1501.44197157651</v>
+      </c>
+      <c r="F35">
+        <v>58.702051599754597</v>
+      </c>
+      <c r="G35">
+        <v>32.894521565778</v>
+      </c>
+      <c r="H35">
+        <v>1.4413400382107899</v>
+      </c>
+      <c r="I35">
+        <v>3573.23614738063</v>
+      </c>
+      <c r="J35">
+        <v>43.861523471265599</v>
+      </c>
+      <c r="K35">
+        <v>0.60617142719112505</v>
+      </c>
+      <c r="L35">
+        <v>6.0109502426272499E-2</v>
+      </c>
+      <c r="M35">
+        <v>9526.4498453900105</v>
+      </c>
+      <c r="N35">
+        <v>732.87865686527698</v>
+      </c>
+      <c r="O35">
+        <v>0.90756886586298002</v>
+      </c>
+      <c r="P35">
+        <v>6.5172174766579202E-3</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>55</v>
+      </c>
+      <c r="R35" t="s">
+        <v>55</v>
+      </c>
+      <c r="S35">
+        <v>3.8330315481361898</v>
+      </c>
+      <c r="T35">
+        <v>0.17256005241428199</v>
+      </c>
+      <c r="U35">
+        <v>1.02722177064887</v>
+      </c>
+      <c r="V35">
+        <v>26.757023416967598</v>
+      </c>
+      <c r="W35">
+        <v>26.548922041323301</v>
+      </c>
+      <c r="X35">
+        <v>146.13520809501901</v>
+      </c>
+      <c r="Z35">
+        <v>0.95701280289892898</v>
+      </c>
+      <c r="AA35">
+        <v>0.20033688063119701</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36">
+        <v>107</v>
+      </c>
+      <c r="C36">
+        <v>0.25390865557877501</v>
+      </c>
+      <c r="D36">
+        <v>1.39742537432442E-2</v>
+      </c>
+      <c r="E36">
+        <v>1456.7171111585601</v>
+      </c>
+      <c r="F36">
+        <v>71.367388171121604</v>
+      </c>
+      <c r="G36">
+        <v>31.616430531501699</v>
+      </c>
+      <c r="H36">
+        <v>1.6894600360774601</v>
+      </c>
+      <c r="I36">
+        <v>3532.12110329713</v>
+      </c>
+      <c r="J36">
+        <v>51.638160331970703</v>
+      </c>
+      <c r="K36">
+        <v>0.57767156575728895</v>
+      </c>
+      <c r="L36">
+        <v>6.6049668183361193E-2</v>
+      </c>
+      <c r="M36">
+        <v>9143.6036307871309</v>
+      </c>
+      <c r="N36">
+        <v>831.395198091579</v>
+      </c>
+      <c r="O36">
+        <v>0.90168164640433901</v>
+      </c>
+      <c r="P36">
+        <v>8.9269448650129406E-3</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>55</v>
+      </c>
+      <c r="R36" t="s">
+        <v>55</v>
+      </c>
+      <c r="S36">
+        <v>3.9828256330482601</v>
+      </c>
+      <c r="T36">
+        <v>0.21211646861314601</v>
+      </c>
+      <c r="U36">
+        <v>0.98864010958654402</v>
+      </c>
+      <c r="V36">
+        <v>27.332538924511798</v>
+      </c>
+      <c r="W36">
+        <v>28.347237031989501</v>
+      </c>
+      <c r="X36">
+        <v>149.941140011736</v>
+      </c>
+      <c r="Z36">
+        <v>0.84993812930119494</v>
+      </c>
+      <c r="AA36">
+        <v>-6.0718585242599599E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37">
+        <v>108</v>
+      </c>
+      <c r="C37">
+        <v>0.26927445533059602</v>
+      </c>
+      <c r="D37">
+        <v>1.43738226333281E-2</v>
+      </c>
+      <c r="E37">
+        <v>1535.2763327191601</v>
+      </c>
+      <c r="F37">
+        <v>72.466629986174297</v>
+      </c>
+      <c r="G37">
+        <v>33.516667129494003</v>
+      </c>
+      <c r="H37">
+        <v>1.89233585113317</v>
+      </c>
+      <c r="I37">
+        <v>3589.228965499</v>
+      </c>
+      <c r="J37">
+        <v>54.670879433299298</v>
+      </c>
+      <c r="K37">
+        <v>0.56875390728731401</v>
+      </c>
+      <c r="L37">
+        <v>4.44062326753158E-2</v>
+      </c>
+      <c r="M37">
+        <v>9074.1574772876993</v>
+      </c>
+      <c r="N37">
+        <v>573.67698458703501</v>
+      </c>
+      <c r="O37">
+        <v>0.89965794000847099</v>
+      </c>
+      <c r="P37">
+        <v>7.5449096899845997E-3</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>55</v>
+      </c>
+      <c r="R37" t="s">
+        <v>55</v>
+      </c>
+      <c r="S37">
+        <v>3.7498342776312299</v>
+      </c>
+      <c r="T37">
+        <v>0.19267626398472901</v>
+      </c>
+      <c r="U37">
+        <v>0.93617772607528504</v>
+      </c>
+      <c r="V37">
+        <v>26.8641005471532</v>
+      </c>
+      <c r="W37">
+        <v>29.020220431493598</v>
+      </c>
+      <c r="X37">
+        <v>150.505319004341</v>
+      </c>
+      <c r="Z37">
+        <v>0.89712118945643604</v>
+      </c>
+      <c r="AA37">
+        <v>0.281132460713508</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B38">
+        <v>109</v>
+      </c>
+      <c r="C38">
+        <v>0.25968282077357202</v>
+      </c>
+      <c r="D38">
+        <v>1.1991756872003901E-2</v>
+      </c>
+      <c r="E38">
+        <v>1486.90662166278</v>
+      </c>
+      <c r="F38">
+        <v>61.294231242255698</v>
+      </c>
+      <c r="G38">
+        <v>32.487004361015302</v>
+      </c>
+      <c r="H38">
+        <v>1.4484831197297099</v>
+      </c>
+      <c r="I38">
+        <v>3560.9088480866699</v>
+      </c>
+      <c r="J38">
+        <v>43.858032558555003</v>
+      </c>
+      <c r="K38">
+        <v>0.55747394824499796</v>
+      </c>
+      <c r="L38">
+        <v>3.79618434542296E-2</v>
+      </c>
+      <c r="M38">
+        <v>8937.8550652572303</v>
+      </c>
+      <c r="N38">
+        <v>486.55519544719601</v>
+      </c>
+      <c r="O38">
+        <v>0.90460608932249698</v>
+      </c>
+      <c r="P38">
+        <v>6.2449977394794503E-3</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>55</v>
+      </c>
+      <c r="R38" t="s">
+        <v>55</v>
+      </c>
+      <c r="S38">
+        <v>3.8782559444020301</v>
+      </c>
+      <c r="T38">
+        <v>0.18002010934459201</v>
+      </c>
+      <c r="U38">
+        <v>0.97480700332188397</v>
+      </c>
+      <c r="V38">
+        <v>27.383513548495099</v>
+      </c>
+      <c r="W38">
+        <v>28.594734699249699</v>
+      </c>
+      <c r="X38">
+        <v>148.34354319526901</v>
+      </c>
+      <c r="Z38">
+        <v>0.98515542017560698</v>
+      </c>
+      <c r="AA38">
+        <v>2.7375291402949101E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B39">
+        <v>110</v>
+      </c>
+      <c r="C39">
+        <v>0.26086625065941599</v>
+      </c>
+      <c r="D39">
+        <v>9.7535870064367793E-3</v>
+      </c>
+      <c r="E39">
+        <v>1493.4036545566801</v>
+      </c>
+      <c r="F39">
+        <v>49.895897995769602</v>
+      </c>
+      <c r="G39">
+        <v>32.756548958683901</v>
+      </c>
+      <c r="H39">
+        <v>1.31611521236686</v>
+      </c>
+      <c r="I39">
+        <v>3569.8302507072199</v>
+      </c>
+      <c r="J39">
+        <v>39.649790800957099</v>
+      </c>
+      <c r="K39">
+        <v>0.56276422865499098</v>
+      </c>
+      <c r="L39">
+        <v>3.8601735378481702E-2</v>
+      </c>
+      <c r="M39">
+        <v>9005.2314532240598</v>
+      </c>
+      <c r="N39">
+        <v>505.71327294786101</v>
+      </c>
+      <c r="O39">
+        <v>0.90702731862335395</v>
+      </c>
+      <c r="P39">
+        <v>8.0433516559248602E-3</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S39">
+        <v>3.8481566856773202</v>
+      </c>
+      <c r="T39">
+        <v>0.145254163200672</v>
+      </c>
+      <c r="U39">
+        <v>0.97823000332825005</v>
+      </c>
+      <c r="V39">
+        <v>26.5092329322041</v>
+      </c>
+      <c r="W39">
+        <v>26.657560834433198</v>
+      </c>
+      <c r="X39">
+        <v>145.03768370697199</v>
+      </c>
+      <c r="Z39">
+        <v>0.90541863442986203</v>
+      </c>
+      <c r="AA39">
+        <v>-5.5917152470779899E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B40">
+        <v>96</v>
+      </c>
+      <c r="C40">
+        <v>0.27205015887866502</v>
+      </c>
+      <c r="D40">
+        <v>9.4559823124843508E-3</v>
+      </c>
+      <c r="E40">
+        <v>1550.39633831724</v>
+      </c>
+      <c r="F40">
+        <v>48.0169459592679</v>
+      </c>
+      <c r="G40">
+        <v>33.920577724191801</v>
+      </c>
+      <c r="H40">
+        <v>1.23095903638533</v>
+      </c>
+      <c r="I40">
+        <v>3604.8392486778298</v>
+      </c>
+      <c r="J40">
+        <v>36.329976271339198</v>
+      </c>
+      <c r="K40">
+        <v>0.54081521760176099</v>
+      </c>
+      <c r="L40">
+        <v>3.6237443598639701E-2</v>
+      </c>
+      <c r="M40">
+        <v>8721.6567427549708</v>
+      </c>
+      <c r="N40">
+        <v>476.92649981848302</v>
+      </c>
+      <c r="O40">
+        <v>0.90881299832264395</v>
+      </c>
+      <c r="P40">
+        <v>7.32916892588631E-3</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>55</v>
+      </c>
+      <c r="R40" t="s">
+        <v>55</v>
+      </c>
+      <c r="S40">
+        <v>3.6847534956912198</v>
+      </c>
+      <c r="T40">
+        <v>0.13153016981403501</v>
+      </c>
+      <c r="U40">
+        <v>0.88117777300713296</v>
+      </c>
+      <c r="V40">
+        <v>26.216307668238102</v>
+      </c>
+      <c r="W40">
+        <v>29.626790567325902</v>
+      </c>
+      <c r="X40">
+        <v>149.30367712172099</v>
+      </c>
+      <c r="Z40">
+        <v>0.89897369412408101</v>
+      </c>
+      <c r="AA40">
+        <v>-0.62479420315952106</v>
+      </c>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B41">
+        <v>97</v>
+      </c>
+      <c r="C41">
+        <v>0.26296977592390602</v>
+      </c>
+      <c r="D41">
+        <v>8.89984985089292E-3</v>
+      </c>
+      <c r="E41">
+        <v>1504.29484282051</v>
+      </c>
+      <c r="F41">
+        <v>45.562841604131201</v>
+      </c>
+      <c r="G41">
+        <v>33.039319678420298</v>
+      </c>
+      <c r="H41">
+        <v>1.0692331668336099</v>
+      </c>
+      <c r="I41">
+        <v>3579.46677255144</v>
+      </c>
+      <c r="J41">
+        <v>32.524884321129399</v>
+      </c>
+      <c r="K41">
+        <v>0.52415686409123197</v>
+      </c>
+      <c r="L41">
+        <v>3.5339190514498298E-2</v>
+      </c>
+      <c r="M41">
+        <v>8502.3081833894503</v>
+      </c>
+      <c r="N41">
+        <v>469.90241789443701</v>
+      </c>
+      <c r="O41">
+        <v>0.915665609218836</v>
+      </c>
+      <c r="P41">
+        <v>9.0033617729332101E-3</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>55</v>
+      </c>
+      <c r="R41" t="s">
+        <v>55</v>
+      </c>
+      <c r="S41">
+        <v>3.8112254722418002</v>
+      </c>
+      <c r="T41">
+        <v>0.13336638849166699</v>
+      </c>
+      <c r="U41">
+        <v>0.88957465643790101</v>
+      </c>
+      <c r="V41">
+        <v>27.603355388871101</v>
+      </c>
+      <c r="W41">
+        <v>30.784972814648398</v>
+      </c>
+      <c r="X41">
+        <v>150.304786288325</v>
+      </c>
+      <c r="Z41">
+        <v>0.91315153325116905</v>
+      </c>
+      <c r="AA41">
+        <v>0.53639485063033598</v>
+      </c>
+    </row>
+    <row r="42" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B42">
+        <v>98</v>
+      </c>
+      <c r="C42">
+        <v>0.27102217802852702</v>
+      </c>
+      <c r="D42">
+        <v>1.19445967953E-2</v>
+      </c>
+      <c r="E42">
+        <v>1544.7177672043999</v>
+      </c>
+      <c r="F42">
+        <v>60.2152751011877</v>
+      </c>
+      <c r="G42">
+        <v>34.041871630803897</v>
+      </c>
+      <c r="H42">
+        <v>1.4750536563782699</v>
+      </c>
+      <c r="I42">
+        <v>3607.3200691685201</v>
+      </c>
+      <c r="J42">
+        <v>41.866057196340599</v>
+      </c>
+      <c r="K42">
+        <v>0.56120386626457497</v>
+      </c>
+      <c r="L42">
+        <v>4.1779944513267497E-2</v>
+      </c>
+      <c r="M42">
+        <v>8980.0995866281592</v>
+      </c>
+      <c r="N42">
+        <v>546.98757940177495</v>
+      </c>
+      <c r="O42">
+        <v>0.91480173642996299</v>
+      </c>
+      <c r="P42">
+        <v>1.00594578561764E-2</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>55</v>
+      </c>
+      <c r="R42" t="s">
+        <v>55</v>
+      </c>
+      <c r="S42">
+        <v>3.7095496290515402</v>
+      </c>
+      <c r="T42">
+        <v>0.15795439881106299</v>
+      </c>
+      <c r="U42">
+        <v>0.92606904987795002</v>
+      </c>
+      <c r="V42">
+        <v>26.241312932773699</v>
+      </c>
+      <c r="W42">
+        <v>28.240996256503301</v>
+      </c>
+      <c r="X42">
+        <v>151.417679564195</v>
+      </c>
+      <c r="Z42">
+        <v>0.88835512676806705</v>
+      </c>
+      <c r="AA42">
+        <v>5.1110500770787999E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B43">
+        <v>99</v>
+      </c>
+      <c r="C43">
+        <v>0.27324554362878301</v>
+      </c>
+      <c r="D43">
+        <v>1.0699789775050201E-2</v>
+      </c>
+      <c r="E43">
+        <v>1556.2333139413499</v>
+      </c>
+      <c r="F43">
+        <v>54.072415708923302</v>
+      </c>
+      <c r="G43">
+        <v>34.229671208327098</v>
+      </c>
+      <c r="H43">
+        <v>1.2920525691720499</v>
+      </c>
+      <c r="I43">
+        <v>3613.6055685819902</v>
+      </c>
+      <c r="J43">
+        <v>37.284832530073601</v>
+      </c>
+      <c r="K43">
+        <v>0.56117199655500405</v>
+      </c>
+      <c r="L43">
+        <v>3.8388147369305098E-2</v>
+      </c>
+      <c r="M43">
+        <v>8985.0732895479196</v>
+      </c>
+      <c r="N43">
+        <v>498.80453235211399</v>
+      </c>
+      <c r="O43">
+        <v>0.91174007037316396</v>
+      </c>
+      <c r="P43">
+        <v>7.7844019840020602E-3</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>55</v>
+      </c>
+      <c r="R43" t="s">
+        <v>55</v>
+      </c>
+      <c r="S43">
+        <v>3.6738873254079798</v>
+      </c>
+      <c r="T43">
+        <v>0.14370807344665801</v>
+      </c>
+      <c r="U43">
+        <v>0.91247557794668699</v>
+      </c>
+      <c r="V43">
+        <v>26.338474694178</v>
+      </c>
+      <c r="W43">
+        <v>27.9970964784128</v>
+      </c>
+      <c r="X43">
+        <v>155.486909209906</v>
+      </c>
+      <c r="Z43">
+        <v>0.70690260888925904</v>
+      </c>
+      <c r="AA43">
+        <v>-0.16247719575806999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B44">
+        <v>16</v>
+      </c>
+      <c r="C44">
+        <v>0.73467077100251299</v>
+      </c>
+      <c r="D44">
+        <v>1.10436096029175E-2</v>
+      </c>
+      <c r="E44">
+        <v>3550.2109255257801</v>
+      </c>
+      <c r="F44">
+        <v>41.031762546597498</v>
+      </c>
+      <c r="G44">
+        <v>30.524060357381298</v>
+      </c>
+      <c r="H44">
+        <v>0.46188173014537098</v>
+      </c>
+      <c r="I44">
+        <v>3503.3421774799399</v>
+      </c>
+      <c r="J44">
+        <v>14.9129622955831</v>
+      </c>
+      <c r="K44">
+        <v>0.18336571502457699</v>
+      </c>
+      <c r="L44">
+        <v>8.6950696780415705E-3</v>
+      </c>
+      <c r="M44">
+        <v>3402.2621515053002</v>
+      </c>
+      <c r="N44">
+        <v>148.49611542010999</v>
+      </c>
+      <c r="O44">
+        <v>0.301857903247437</v>
+      </c>
+      <c r="P44">
+        <v>9.5515053423811695E-4</v>
+      </c>
+      <c r="Q44">
+        <v>3479.04837876172</v>
+      </c>
+      <c r="R44">
+        <v>4.8976800082038103</v>
+      </c>
+      <c r="S44">
+        <v>1.3585849311460001</v>
+      </c>
+      <c r="T44">
+        <v>2.0419002137143E-2</v>
+      </c>
+      <c r="U44">
+        <v>0.92031813418720498</v>
+      </c>
+      <c r="V44">
+        <v>166.11189400185199</v>
+      </c>
+      <c r="W44">
+        <v>178.17279940513399</v>
+      </c>
+      <c r="X44">
+        <v>305.472724604794</v>
+      </c>
+      <c r="Z44">
+        <v>0.92955667262784403</v>
+      </c>
+      <c r="AA44">
+        <v>-8.0338690608449004E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45">
+        <v>17</v>
+      </c>
+      <c r="C45">
+        <v>0.73318330247486496</v>
+      </c>
+      <c r="D45">
+        <v>1.36339546257717E-2</v>
+      </c>
+      <c r="E45">
+        <v>3544.3788628941002</v>
+      </c>
+      <c r="F45">
+        <v>50.375432891292697</v>
+      </c>
+      <c r="G45">
+        <v>30.489243414009401</v>
+      </c>
+      <c r="H45">
+        <v>0.58633380708169902</v>
+      </c>
+      <c r="I45">
+        <v>3501.9350366746798</v>
+      </c>
+      <c r="J45">
+        <v>18.6372431487945</v>
+      </c>
+      <c r="K45">
+        <v>0.18643018366844299</v>
+      </c>
+      <c r="L45">
+        <v>8.6910135526581094E-3</v>
+      </c>
+      <c r="M45">
+        <v>3454.6014902664001</v>
+      </c>
+      <c r="N45">
+        <v>147.955468194362</v>
+      </c>
+      <c r="O45">
+        <v>0.300921818341644</v>
+      </c>
+      <c r="P45">
+        <v>6.58416199630359E-4</v>
+      </c>
+      <c r="Q45">
+        <v>3474.2599070814999</v>
+      </c>
+      <c r="R45">
+        <v>3.3849775887960001</v>
+      </c>
+      <c r="S45">
+        <v>1.3623974136101</v>
+      </c>
+      <c r="T45">
+        <v>2.45843338992798E-2</v>
+      </c>
+      <c r="U45">
+        <v>1.07909477537854</v>
+      </c>
+      <c r="V45">
+        <v>185.018039621475</v>
+      </c>
+      <c r="W45">
+        <v>170.63256330341699</v>
+      </c>
+      <c r="X45">
+        <v>303.08674382347198</v>
+      </c>
+      <c r="Z45">
+        <v>0.93117267011921301</v>
+      </c>
+      <c r="AA45">
+        <v>2.8247347050086202E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B46">
+        <v>16</v>
+      </c>
+      <c r="C46">
+        <v>9.3320480725604699E-2</v>
+      </c>
+      <c r="D46">
+        <v>3.7048524908506598E-3</v>
+      </c>
+      <c r="E46">
+        <v>574.97864050461999</v>
+      </c>
+      <c r="F46">
+        <v>21.832143263091901</v>
+      </c>
+      <c r="G46">
+        <v>0.75141078797658101</v>
+      </c>
+      <c r="H46">
+        <v>3.5215260023404499E-2</v>
+      </c>
+      <c r="I46">
+        <v>568.10514783875794</v>
+      </c>
+      <c r="J46">
+        <v>20.646821912390301</v>
+      </c>
+      <c r="K46">
+        <v>3.3542409077921699E-2</v>
+      </c>
+      <c r="L46">
+        <v>6.6439188738460601E-3</v>
+      </c>
+      <c r="M46">
+        <v>665.06437171016705</v>
+      </c>
+      <c r="N46">
+        <v>128.98291479948199</v>
+      </c>
+      <c r="O46">
+        <v>5.8541074528562997E-2</v>
+      </c>
+      <c r="P46">
+        <v>1.5842282651840501E-3</v>
+      </c>
+      <c r="Q46">
+        <v>544.08985371574499</v>
+      </c>
+      <c r="R46">
+        <v>59.770789303264898</v>
+      </c>
+      <c r="S46">
+        <v>10.7602792185805</v>
+      </c>
+      <c r="T46">
+        <v>0.428559191706742</v>
+      </c>
+      <c r="U46">
+        <v>8.4167765242117891</v>
+      </c>
+      <c r="V46">
+        <v>85.024175966472299</v>
+      </c>
+      <c r="W46">
+        <v>11.040611234208701</v>
+      </c>
+      <c r="X46">
+        <v>3.2587080607743801</v>
+      </c>
+      <c r="Z46">
+        <v>0.915979846426349</v>
+      </c>
+      <c r="AA46">
+        <v>-0.15245831769646101</v>
+      </c>
+    </row>
+    <row r="47" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B47">
+        <v>17</v>
+      </c>
+      <c r="C47">
+        <v>9.1105410350207097E-2</v>
+      </c>
+      <c r="D47">
+        <v>2.2455284437826501E-3</v>
+      </c>
+      <c r="E47">
+        <v>562.00993520417398</v>
+      </c>
+      <c r="F47">
+        <v>13.2661485511018</v>
+      </c>
+      <c r="G47">
+        <v>0.74681964854685201</v>
+      </c>
+      <c r="H47">
+        <v>3.4782934530353603E-2</v>
+      </c>
+      <c r="I47">
+        <v>565.48809766868101</v>
+      </c>
+      <c r="J47">
+        <v>19.9452436827195</v>
+      </c>
+      <c r="K47">
+        <v>3.7161724355241302E-2</v>
+      </c>
+      <c r="L47">
+        <v>6.3825565843194897E-3</v>
+      </c>
+      <c r="M47">
+        <v>735.88431786368801</v>
+      </c>
+      <c r="N47">
+        <v>123.659269823803</v>
+      </c>
+      <c r="O47">
+        <v>5.9250623192071999E-2</v>
+      </c>
+      <c r="P47">
+        <v>1.54017217254202E-3</v>
+      </c>
+      <c r="Q47">
+        <v>570.91727265606596</v>
+      </c>
+      <c r="R47">
+        <v>55.617607144597798</v>
+      </c>
+      <c r="S47">
+        <v>10.977120723343299</v>
+      </c>
+      <c r="T47">
+        <v>0.27209641532610601</v>
+      </c>
+      <c r="U47">
+        <v>8.8473565976114195</v>
+      </c>
+      <c r="V47">
+        <v>85.2720722063099</v>
+      </c>
+      <c r="W47">
+        <v>10.550057479350601</v>
+      </c>
+      <c r="X47">
+        <v>3.3202213433148402</v>
+      </c>
+      <c r="Z47">
+        <v>0.94089878006680805</v>
+      </c>
+      <c r="AA47">
+        <v>0.31007118952537499</v>
+      </c>
+    </row>
+    <row r="48" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B48">
+        <v>16</v>
+      </c>
+      <c r="C48">
+        <v>5.3168736256061597E-2</v>
+      </c>
+      <c r="D48">
+        <v>7.39025348781407E-4</v>
+      </c>
+      <c r="E48">
+        <v>333.93944114441899</v>
+      </c>
+      <c r="F48">
+        <v>4.5234091499474998</v>
+      </c>
+      <c r="G48">
+        <v>0.38703108466123998</v>
+      </c>
+      <c r="H48">
+        <v>6.4991702149753304E-3</v>
+      </c>
+      <c r="I48">
+        <v>332.147970392133</v>
+      </c>
+      <c r="J48">
+        <v>4.7739488832900099</v>
+      </c>
+      <c r="K48">
+        <v>1.52868603988834E-2</v>
+      </c>
+      <c r="L48">
+        <v>8.9672541900202201E-4</v>
+      </c>
+      <c r="M48">
+        <v>306.62451864654201</v>
+      </c>
+      <c r="N48">
+        <v>17.854018287188001</v>
+      </c>
+      <c r="O48">
+        <v>5.3034163001059301E-2</v>
+      </c>
+      <c r="P48">
+        <v>6.9701519454669195E-4</v>
+      </c>
+      <c r="Q48">
+        <v>328.01361591262503</v>
+      </c>
+      <c r="R48">
+        <v>29.575827884627898</v>
+      </c>
+      <c r="S48">
+        <v>18.766282067353298</v>
+      </c>
+      <c r="T48">
+        <v>0.26136454579177898</v>
+      </c>
+      <c r="U48">
+        <v>9.8646240233265008</v>
+      </c>
+      <c r="V48">
+        <v>615.94384944245996</v>
+      </c>
+      <c r="W48">
+        <v>61.871160760818903</v>
+      </c>
+      <c r="X48">
+        <v>8.8297682303217009</v>
+      </c>
+      <c r="Z48">
+        <v>0.89968698888305798</v>
+      </c>
+      <c r="AA48">
+        <v>0.45695331132832201</v>
+      </c>
+    </row>
+    <row r="49" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B49">
+        <v>17</v>
+      </c>
+      <c r="C49">
+        <v>5.3768300340449701E-2</v>
+      </c>
+      <c r="D49">
+        <v>9.8884379150424007E-4</v>
+      </c>
+      <c r="E49">
+        <v>337.60268594355</v>
+      </c>
+      <c r="F49">
+        <v>6.0471994122348898</v>
+      </c>
+      <c r="G49">
+        <v>0.39241869287406</v>
+      </c>
+      <c r="H49">
+        <v>6.7055565943890403E-3</v>
+      </c>
+      <c r="I49">
+        <v>336.08193919516202</v>
+      </c>
+      <c r="J49">
+        <v>4.8774298082930496</v>
+      </c>
+      <c r="K49">
+        <v>1.6272305320609099E-2</v>
+      </c>
+      <c r="L49">
+        <v>8.4267315855483804E-4</v>
+      </c>
+      <c r="M49">
+        <v>326.23950540444798</v>
+      </c>
+      <c r="N49">
+        <v>16.753357880505099</v>
+      </c>
+      <c r="O49">
+        <v>5.2985417652288702E-2</v>
+      </c>
+      <c r="P49">
+        <v>7.72815350740274E-4</v>
+      </c>
+      <c r="Q49">
+        <v>325.61323208262502</v>
+      </c>
+      <c r="R49">
+        <v>33.339564432830898</v>
+      </c>
+      <c r="S49">
+        <v>18.574015202967502</v>
+      </c>
+      <c r="T49">
+        <v>0.33756401991449397</v>
+      </c>
+      <c r="U49">
+        <v>9.3140345044565098</v>
+      </c>
+      <c r="V49">
+        <v>770.17646138429404</v>
+      </c>
+      <c r="W49">
+        <v>80.843976659903504</v>
+      </c>
+      <c r="X49">
+        <v>11.7459699438639</v>
+      </c>
+      <c r="Z49">
+        <v>0.74096840257228003</v>
+      </c>
+      <c r="AA49">
+        <v>-7.9025364954862704E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B50">
+        <v>18</v>
+      </c>
+      <c r="C50">
+        <v>5.29007004885318E-2</v>
+      </c>
+      <c r="D50">
+        <v>1.11112554436586E-3</v>
+      </c>
+      <c r="E50">
+        <v>332.28868453498501</v>
+      </c>
+      <c r="F50">
+        <v>6.8029977050076997</v>
+      </c>
+      <c r="G50">
+        <v>0.38387454959931699</v>
+      </c>
+      <c r="H50">
+        <v>8.0918226719717094E-3</v>
+      </c>
+      <c r="I50">
+        <v>329.80259484470298</v>
+      </c>
+      <c r="J50">
+        <v>5.93301683278567</v>
+      </c>
+      <c r="K50">
+        <v>1.5359249681679401E-2</v>
+      </c>
+      <c r="L50">
+        <v>8.1422502804655598E-4</v>
+      </c>
+      <c r="M50">
+        <v>308.071255801939</v>
+      </c>
+      <c r="N50">
+        <v>16.211682390538101</v>
+      </c>
+      <c r="O50">
+        <v>5.2460499923987901E-2</v>
+      </c>
+      <c r="P50">
+        <v>6.6170846663028704E-4</v>
+      </c>
+      <c r="Q50">
+        <v>303.28386969040298</v>
+      </c>
+      <c r="R50">
+        <v>29.007273791172199</v>
+      </c>
+      <c r="S50">
+        <v>18.895304497052901</v>
+      </c>
+      <c r="T50">
+        <v>0.39842350008884903</v>
+      </c>
+      <c r="U50">
+        <v>9.5906145780561705</v>
+      </c>
+      <c r="V50">
+        <v>728.06464290535496</v>
+      </c>
+      <c r="W50">
+        <v>75.982543179817796</v>
+      </c>
+      <c r="X50">
+        <v>11.039000791351601</v>
+      </c>
+      <c r="Z50">
+        <v>0.92621016479573504</v>
+      </c>
+      <c r="AA50">
+        <v>-0.114202582488052</v>
       </c>
     </row>
   </sheetData>

</xml_diff>